<commit_message>
update : data files
</commit_message>
<xml_diff>
--- a/cad-tracker/SampleData1.xlsx
+++ b/cad-tracker/SampleData1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Projects  (Industry)\CAD automation implementation\cad-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F615B5E9-5ABB-4563-A084-10EE2E20C04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A4ADC7-38E1-4DBE-B56C-3DD552B4D26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EF7BFDF4-3805-439A-8D98-AB2AEA4383B5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{EF7BFDF4-3805-439A-8D98-AB2AEA4383B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -119,93 +119,12 @@
   </si>
   <si>
     <t>December 28,2021</t>
-  </si>
-  <si>
-    <t>Date1</t>
-  </si>
-  <si>
-    <t>CstName1</t>
-  </si>
-  <si>
-    <t>CstAddressOne1</t>
-  </si>
-  <si>
-    <t>CstAddressTwo1</t>
-  </si>
-  <si>
-    <t>VehicleMade1</t>
-  </si>
-  <si>
-    <t>VehicleNum1</t>
-  </si>
-  <si>
-    <t>VehicleModel1</t>
-  </si>
-  <si>
-    <t>ChasNo1</t>
-  </si>
-  <si>
-    <t>EngNo1</t>
-  </si>
-  <si>
-    <t>YOM1</t>
-  </si>
-  <si>
-    <t>DmSum1</t>
-  </si>
-  <si>
-    <t>RSUM1</t>
-  </si>
-  <si>
-    <t>SetDate1</t>
-  </si>
-  <si>
-    <t>fvd</t>
-  </si>
-  <si>
-    <t>ereff</t>
-  </si>
-  <si>
-    <t>dgerg</t>
-  </si>
-  <si>
-    <t>dfbfbfb</t>
-  </si>
-  <si>
-    <t>rgfdfbdf</t>
-  </si>
-  <si>
-    <t>gdfbdfbd</t>
-  </si>
-  <si>
-    <t>gsdgsdg</t>
-  </si>
-  <si>
-    <t>sdfsdfsdf</t>
-  </si>
-  <si>
-    <t>dfgdfgdfg</t>
-  </si>
-  <si>
-    <t>dsfdfsd</t>
-  </si>
-  <si>
-    <t>fbdfbdfb</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>ggabdg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -255,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -265,12 +184,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,11 +501,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FFCF893-15BB-4534-B97A-6F25E0D70F73}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C476CE66-BED4-46C2-8859-4D28511D1C87}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B965A3-11D5-4239-8414-BD4E52939FD5}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -601,7 +532,8 @@
     <col min="6" max="7" width="15.88671875" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -614,133 +546,7 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="3">
-        <v>2312</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="7">
-        <v>2342</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" s="5">
-        <v>12323</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B965A3-11D5-4239-8414-BD4E52939FD5}">
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -790,7 +596,7 @@
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E2" t="s">
@@ -814,7 +620,7 @@
       <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="M2">
@@ -823,7 +629,7 @@
       <c r="N2" s="8">
         <v>7150000</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="8">
         <v>420000</v>
       </c>
       <c r="P2" t="s">

</xml_diff>

<commit_message>
update : bugs fixed
</commit_message>
<xml_diff>
--- a/cad-tracker/SampleData1.xlsx
+++ b/cad-tracker/SampleData1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Projects  (Industry)\CAD automation implementation\cad-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A4ADC7-38E1-4DBE-B56C-3DD552B4D26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6589A59-9B7B-49CB-9DBA-FA959915D38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{EF7BFDF4-3805-439A-8D98-AB2AEA4383B5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EF7BFDF4-3805-439A-8D98-AB2AEA4383B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B965A3-11D5-4239-8414-BD4E52939FD5}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
fixed : fixed bugs
</commit_message>
<xml_diff>
--- a/cad-tracker/SampleData1.xlsx
+++ b/cad-tracker/SampleData1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Projects  (Industry)\CAD automation implementation\cad-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245E1DB9-D039-4D3D-B81B-27E426F6AC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABF880C-5031-493A-9467-D4F25569F789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -769,10 +769,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278CECC8-1364-45B0-AC62-887AE8A6C17F}">
-  <dimension ref="A1:AQ2"/>
+  <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -817,12 +817,11 @@
     <col min="38" max="38" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="2" customFormat="1">
+    <row r="1" spans="1:42" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -944,16 +943,13 @@
         <v>76</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:42">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1074,10 +1070,7 @@
       <c r="AN2">
         <v>11000000</v>
       </c>
-      <c r="AO2">
-        <v>10000000</v>
-      </c>
-      <c r="AP2" t="s">
+      <c r="AO2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>